<commit_message>
Revisão geral no GQA
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Genérico/7-Garantia da Qualidade/Templates/Registro de Não Conformidade.xlsx
+++ b/Artefatos de Documentação/Processo Genérico/7-Garantia da Qualidade/Templates/Registro de Não Conformidade.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Data de Abertura</t>
   </si>
@@ -37,9 +35,6 @@
   </si>
   <si>
     <t>Relatada</t>
-  </si>
-  <si>
-    <t>Nº  do Comunicado</t>
   </si>
   <si>
     <t>Área</t>
@@ -450,193 +445,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E16" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="7" width="20.7109375" customWidth="1"/>
+    <col min="1" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="2"/>
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7">
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7">
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7">
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
 </file>
</xml_diff>